<commit_message>
Add Changes to easy ship report
</commit_message>
<xml_diff>
--- a/data/temp_master.xlsx
+++ b/data/temp_master.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="176">
   <si>
     <t>Name</t>
   </si>
@@ -528,6 +528,18 @@
   <si>
     <t>B0FBJ2V43Y</t>
   </si>
+  <si>
+    <t>Makai Atta</t>
+  </si>
+  <si>
+    <t>B0FBKFHQ44</t>
+  </si>
+  <si>
+    <t>B0FBKDTM51</t>
+  </si>
+  <si>
+    <t>B0FBKDZY5F</t>
+  </si>
 </sst>
 </file>
 
@@ -4668,16 +4680,28 @@
       <c r="Z95" s="7"/>
     </row>
     <row r="96">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
+      <c r="A96" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B96" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="C96" s="19">
+        <v>299.0</v>
+      </c>
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
+      <c r="F96" s="11">
+        <v>1.1124999000076E13</v>
+      </c>
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
-      <c r="I96" s="17"/>
-      <c r="J96" s="15"/>
+      <c r="I96" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="J96" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="K96" s="7"/>
       <c r="L96" s="7"/>
       <c r="M96" s="7"/>
@@ -4696,16 +4720,28 @@
       <c r="Z96" s="7"/>
     </row>
     <row r="97">
-      <c r="A97" s="7"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
+      <c r="A97" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B97" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="C97" s="19">
+        <v>499.0</v>
+      </c>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
-      <c r="F97" s="7"/>
+      <c r="F97" s="11">
+        <v>1.1124999000076E13</v>
+      </c>
       <c r="G97" s="7"/>
       <c r="H97" s="7"/>
-      <c r="I97" s="17"/>
-      <c r="J97" s="15"/>
+      <c r="I97" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="J97" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="K97" s="7"/>
       <c r="L97" s="7"/>
       <c r="M97" s="7"/>
@@ -4724,16 +4760,28 @@
       <c r="Z97" s="7"/>
     </row>
     <row r="98">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
+      <c r="A98" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B98" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="C98" s="19">
+        <v>699.0</v>
+      </c>
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
-      <c r="F98" s="7"/>
+      <c r="F98" s="11">
+        <v>1.1124999000076E13</v>
+      </c>
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
-      <c r="I98" s="17"/>
-      <c r="J98" s="15"/>
+      <c r="I98" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="J98" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="K98" s="7"/>
       <c r="L98" s="7"/>
       <c r="M98" s="7"/>

</xml_diff>